<commit_message>
Started on question 2
</commit_message>
<xml_diff>
--- a/t_test_results.xlsx
+++ b/t_test_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Biomarker</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant</t>
   </si>
   <si>
     <t xml:space="preserve">IL-8</t>
@@ -395,104 +398,134 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>0.329382973552736</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>0.0413896395215315</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="n">
         <v>0.132573767959124</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
         <v>0.0457039171179617</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
         <v>0.251454023156768</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
         <v>0.984880326415234</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="n">
         <v>0.00616650001341388</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
         <v>0.249580861332934</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="n">
         <v>0.00608143105097193</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>